<commit_message>
removing section 3 keys
</commit_message>
<xml_diff>
--- a/03_regression/xlsx/assessment_workbook.xlsx
+++ b/03_regression/xlsx/assessment_workbook.xlsx
@@ -1,37 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phall/workspace/GWU_data_mining/03_regression/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GWU_data_mining\03_regression\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16605"/>
   </bookViews>
   <sheets>
     <sheet name="Lift" sheetId="2" r:id="rId1"/>
     <sheet name="ROC" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>Actual</t>
   </si>
@@ -128,12 +125,15 @@
   <si>
     <t>The better the model, the more area under the ROC curve</t>
   </si>
+  <si>
+    <t>Copyright (C) 2017 J. Patrick Hall, jphall@gwu.edu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +152,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -351,6 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,19 +484,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -499,19 +508,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,19 +553,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -568,19 +577,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.666666666666667</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,11 +604,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2110421152"/>
-        <c:axId val="2110429664"/>
+        <c:axId val="328423128"/>
+        <c:axId val="328426656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2110421152"/>
+        <c:axId val="328423128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,12 +721,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110429664"/>
+        <c:crossAx val="328426656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110429664"/>
+        <c:axId val="328426656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,7 +783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110421152"/>
+        <c:crossAx val="328423128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -970,7 +979,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.8</c:v>
@@ -982,10 +991,10 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -997,13 +1006,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.8</c:v>
@@ -1012,7 +1021,7 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,15 +1036,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2132516544"/>
-        <c:axId val="2133298928"/>
+        <c:axId val="328423912"/>
+        <c:axId val="328424696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2132516544"/>
+        <c:axId val="328423912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
-          <c:min val="0.0"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1151,16 +1160,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133298928"/>
+        <c:crossAx val="328424696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133298928"/>
+        <c:axId val="328424696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
-          <c:min val="0.0"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1271,7 +1280,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132516544"/>
+        <c:crossAx val="328423912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2765,19 +2774,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L27"/>
+  <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2794,7 +2808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>1</v>
       </c>
@@ -2813,7 +2827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>1</v>
       </c>
@@ -2832,7 +2846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -2851,7 +2865,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -2870,7 +2884,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>0</v>
       </c>
@@ -2889,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>1</v>
       </c>
@@ -2897,7 +2911,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>0</v>
       </c>
@@ -2905,7 +2919,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>0</v>
       </c>
@@ -2913,7 +2927,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>0</v>
       </c>
@@ -2921,7 +2935,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>0</v>
       </c>
@@ -2929,29 +2943,29 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>22</v>
       </c>
@@ -2963,17 +2977,17 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>30</v>
       </c>
@@ -2987,18 +3001,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:AM38"/>
+  <dimension ref="B2:AM38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="4" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>2</v>
       </c>
@@ -3018,7 +3041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
@@ -3098,7 +3121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:39" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>1</v>
       </c>
@@ -3178,7 +3201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -3222,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -3302,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>1</v>
       </c>
@@ -3382,7 +3405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>0</v>
       </c>
@@ -3426,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>1</v>
       </c>
@@ -3470,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>0</v>
       </c>
@@ -3556,7 +3579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>0</v>
       </c>
@@ -3642,7 +3665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>0</v>
       </c>
@@ -3686,7 +3709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>0</v>
       </c>
@@ -3736,8 +3759,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>14</v>
       </c>
@@ -3745,7 +3768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
         <v>1</v>
       </c>
@@ -3753,7 +3776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>0.8</v>
       </c>
@@ -3761,7 +3784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>0.6</v>
       </c>
@@ -3769,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>0.2</v>
       </c>
@@ -3777,7 +3800,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>0</v>
       </c>
@@ -3785,7 +3808,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>0</v>
       </c>
@@ -3793,27 +3816,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
         <v>31</v>
       </c>
@@ -3823,6 +3846,7 @@
     <sortCondition descending="1" ref="C3:C12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correct minor typos in lift/roc spreadsheet
</commit_message>
<xml_diff>
--- a/03_regression/xlsx/assessment_workbook.xlsx
+++ b/03_regression/xlsx/assessment_workbook.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GWU_data_mining\03_regression\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phall/workspace/GWU_data_mining/03_regression/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27CCA8D-DB99-2F48-9A21-46D206B5BD67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16605"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lift" sheetId="2" r:id="rId1"/>
     <sheet name="ROC" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,9 +100,6 @@
     <t>Note that the data is sorted by descending probabilities, this is required for lift calculations</t>
   </si>
   <si>
-    <t xml:space="preserve">The divisor for cumulative lift changes because we are acumulating the expected responses and the actual responses </t>
-  </si>
-  <si>
     <t>The divisor for lift is 0.2 because I asked for lift every 20 percentiles; if I draw from the data randomly, I expect to get 20% of the total responses in 20% of the data</t>
   </si>
   <si>
@@ -120,19 +118,22 @@
     <t>We simply plot the values of 1-specificity on the x-axis and sensitivity on the y-axis</t>
   </si>
   <si>
-    <t xml:space="preserve">The better the model, the higher the lift, particulary at low depths </t>
-  </si>
-  <si>
     <t>The better the model, the more area under the ROC curve</t>
   </si>
   <si>
     <t>Copyright (C) 2017 J. Patrick Hall, jphall@gwu.edu</t>
   </si>
+  <si>
+    <t xml:space="preserve">The better the model, the higher the lift, particularly at low depths </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The divisor for cumulative lift changes because we are accumulating the expected responses and the actual responses </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,7 +379,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -422,7 +423,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -526,6 +526,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-993F-1F43-B6B9-80F44B25D004}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -595,6 +600,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-993F-1F43-B6B9-80F44B25D004}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -654,7 +664,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -797,7 +806,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -865,7 +873,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -909,7 +917,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1027,6 +1034,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9A81-014D-B043-86811A6D1478}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1093,7 +1105,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1213,7 +1224,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2458,7 +2468,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2493,7 +2509,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2773,25 +2795,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2808,7 +2830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6">
         <v>1</v>
       </c>
@@ -2827,7 +2849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>1</v>
       </c>
@@ -2846,7 +2868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -2865,7 +2887,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -2884,7 +2906,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>0</v>
       </c>
@@ -2903,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>1</v>
       </c>
@@ -2911,7 +2933,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>0</v>
       </c>
@@ -2919,7 +2941,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>0</v>
       </c>
@@ -2927,7 +2949,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>0</v>
       </c>
@@ -2935,7 +2957,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>0</v>
       </c>
@@ -2943,29 +2965,29 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
         <v>22</v>
       </c>
@@ -2977,19 +2999,19 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3000,28 +3022,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AM38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="4" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>2</v>
       </c>
@@ -3041,7 +3063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
@@ -3121,7 +3143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:39" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6">
         <v>1</v>
       </c>
@@ -3201,7 +3223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -3245,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -3325,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>1</v>
       </c>
@@ -3405,7 +3427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>0</v>
       </c>
@@ -3449,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>1</v>
       </c>
@@ -3493,7 +3515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>0</v>
       </c>
@@ -3579,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>0</v>
       </c>
@@ -3665,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>0</v>
       </c>
@@ -3709,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:39" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>0</v>
       </c>
@@ -3723,44 +3745,44 @@
         <v>1</v>
       </c>
       <c r="H15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>0</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0</v>
+      </c>
+      <c r="W15" s="4">
+        <v>0</v>
+      </c>
+      <c r="X15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>0</v>
-      </c>
-      <c r="R15" s="5">
-        <v>0</v>
-      </c>
-      <c r="W15" s="4">
-        <v>0</v>
-      </c>
-      <c r="X15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AL15" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>14</v>
       </c>
@@ -3768,7 +3790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <v>1</v>
       </c>
@@ -3776,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>0.8</v>
       </c>
@@ -3784,7 +3806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>0.6</v>
       </c>
@@ -3792,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>0.2</v>
       </c>
@@ -3800,7 +3822,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>0</v>
       </c>
@@ -3808,7 +3830,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>0</v>
       </c>
@@ -3816,29 +3838,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="12" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="12" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="12" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>